<commit_message>
fix max pressure reading
</commit_message>
<xml_diff>
--- a/data/Rainfall_Simulator_Calibration.xlsx
+++ b/data/Rainfall_Simulator_Calibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Documents/WUR Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Documents/R_Scripts/TWP_Runoff/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04846BE-8C87-3046-A551-305B022F35FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B84EA0-ACB7-DC42-A742-DA1046C39267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="780" windowWidth="28640" windowHeight="16800" firstSheet="6" activeTab="21" xr2:uid="{E070D50E-D6BF-4C34-AAC0-941B728BAD5B}"/>
+    <workbookView xWindow="21780" yWindow="2800" windowWidth="28640" windowHeight="16800" activeTab="4" xr2:uid="{E070D50E-D6BF-4C34-AAC0-941B728BAD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="44" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="40">
   <si>
     <t>x</t>
   </si>
@@ -134,15 +134,6 @@
     <t>Front</t>
   </si>
   <si>
-    <t>3 bar</t>
-  </si>
-  <si>
-    <t>2.2 bar (fully shut)</t>
-  </si>
-  <si>
-    <t>2.2 bar</t>
-  </si>
-  <si>
     <t>1.5 bar</t>
   </si>
   <si>
@@ -180,6 +171,12 @@
   </si>
   <si>
     <t>high3</t>
+  </si>
+  <si>
+    <t>2.5 bar</t>
+  </si>
+  <si>
+    <t>2.4 bar</t>
   </si>
 </sst>
 </file>
@@ -254,13 +251,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2532,7 +2529,7 @@
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2542,18 +2539,18 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" s="8">
         <f>AVERAGE(med3_1!C26, med3_2!C26, med3_3!C26)</f>
@@ -2566,7 +2563,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <f>AVERAGE(low_1!C26, low_2!C26, low_3!C26)</f>
@@ -2579,7 +2576,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <f>AVERAGE(med_1!C26, med_2!C26, med_3!C26)</f>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8">
         <f>AVERAGE(med2_1!C26, med2_2!C26, med2_3!C26)</f>
@@ -2605,7 +2602,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <f>AVERAGE(high_1!C26, high_2!C26, high_3!C26)</f>
@@ -2618,7 +2615,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8">
         <f>AVERAGE(high2_1!C26, high2_2!C26, high2_3!C26)</f>
@@ -2631,7 +2628,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <f>AVERAGE(high3_1!C26, high3_2!C26, high3_3!C26)</f>
@@ -2663,10 +2660,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2723,7 +2720,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -3109,6 +3106,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -3116,12 +3119,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3144,10 +3141,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -3165,7 +3162,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -3204,7 +3201,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -3590,6 +3587,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -3597,12 +3600,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3625,10 +3622,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -3646,7 +3643,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -3685,7 +3682,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -4071,6 +4068,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -4078,12 +4081,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4106,10 +4103,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4127,7 +4124,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -4166,7 +4163,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -4552,6 +4549,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -4559,12 +4562,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4576,7 +4573,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4587,10 +4584,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4608,7 +4605,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -4647,7 +4644,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -5033,6 +5030,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -5040,12 +5043,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5057,7 +5054,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5068,10 +5065,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -5089,7 +5086,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -5128,7 +5125,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -5514,6 +5511,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -5521,12 +5524,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5538,7 +5535,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5549,10 +5546,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -5570,7 +5567,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -5609,7 +5606,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -5995,6 +5992,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -6002,12 +6005,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6030,10 +6027,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -6090,7 +6087,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -6476,6 +6473,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -6483,12 +6486,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6511,10 +6508,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -6571,7 +6568,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -6957,6 +6954,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -6964,12 +6967,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6992,10 +6989,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -7052,7 +7049,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -7438,6 +7435,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -7445,12 +7448,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7473,10 +7470,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -7494,7 +7491,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -7533,7 +7530,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -7919,6 +7916,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -7926,12 +7929,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7954,10 +7951,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -8014,7 +8011,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -8400,6 +8397,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -8407,12 +8410,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8435,10 +8432,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -8495,7 +8492,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -8881,6 +8878,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -8888,12 +8891,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8904,7 +8901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1654A0A-8AC2-2B46-AF74-2653CEE720C0}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -8916,10 +8913,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -8976,7 +8973,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -9362,11 +9359,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A7:B7"/>
@@ -9375,6 +9367,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9397,10 +9394,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -9418,7 +9415,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -9457,7 +9454,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -9843,6 +9840,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -9850,12 +9853,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9878,10 +9875,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -9899,7 +9896,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -9938,7 +9935,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -10324,6 +10321,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -10331,12 +10334,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10347,8 +10344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF59F8C-13DC-EE44-B839-2B78F635B684}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10359,10 +10356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -10380,7 +10377,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -10419,7 +10416,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -10805,6 +10802,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -10812,12 +10815,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10829,7 +10826,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10840,10 +10837,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -10861,7 +10858,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -10900,7 +10897,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -11286,6 +11283,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -11293,12 +11296,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11310,7 +11307,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11321,10 +11318,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -11342,7 +11339,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -11381,7 +11378,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -11767,6 +11764,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -11774,12 +11777,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11802,10 +11799,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -11862,7 +11859,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -12248,6 +12245,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -12255,12 +12258,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12283,10 +12280,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -12343,7 +12340,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>45784</v>
       </c>
       <c r="D7" s="12"/>
@@ -12729,6 +12726,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:B1"/>
@@ -12736,12 +12739,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>